<commit_message>
Started work on iOS 7
</commit_message>
<xml_diff>
--- a/HHSApp/HHSAPP.xlsx
+++ b/HHSApp/HHSAPP.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="23416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="0" windowWidth="18420" windowHeight="22820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Staff" sheetId="1" r:id="rId1"/>
+    <sheet name=" 2012-2013" sheetId="1" r:id="rId1"/>
+    <sheet name="2013-2014" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="326">
   <si>
     <t>FirstName</t>
   </si>
@@ -934,13 +935,79 @@
   </si>
   <si>
     <t>William.N.Murphy@hanovernorwichschools.org</t>
+  </si>
+  <si>
+    <t>Katie</t>
+  </si>
+  <si>
+    <t>Kara</t>
+  </si>
+  <si>
+    <t>Waters</t>
+  </si>
+  <si>
+    <t>Shannon</t>
+  </si>
+  <si>
+    <t>Pogue</t>
+  </si>
+  <si>
+    <t>Engilsh</t>
+  </si>
+  <si>
+    <t>Brady</t>
+  </si>
+  <si>
+    <t>Eskilson</t>
+  </si>
+  <si>
+    <t>Jarrod</t>
+  </si>
+  <si>
+    <t>Shaheen</t>
+  </si>
+  <si>
+    <t>Warren</t>
+  </si>
+  <si>
+    <t>Tucker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlie </t>
+  </si>
+  <si>
+    <t>Odato</t>
+  </si>
+  <si>
+    <t>Chambers</t>
+  </si>
+  <si>
+    <t>Rachael</t>
+  </si>
+  <si>
+    <t>DiGiovanni</t>
+  </si>
+  <si>
+    <t>Department Coordinator</t>
+  </si>
+  <si>
+    <t>Colin</t>
+  </si>
+  <si>
+    <t>Tindall</t>
+  </si>
+  <si>
+    <t>Becky</t>
+  </si>
+  <si>
+    <t>French</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -963,6 +1030,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -981,7 +1056,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1009,12 +1084,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1041,6 +1122,12 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1311,7 +1398,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1321,8 +1408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C52" sqref="A1:G122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3761,4 +3848,2441 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G122"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A120" sqref="A120:XFD120"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="41.6640625" customWidth="1"/>
+    <col min="6" max="6" width="86.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="str">
+        <f>A2&amp;"."&amp;B2&amp;"@hanovernorwichschools.org"</f>
+        <v>Justin.Campbell@hanovernorwichschools.org</v>
+      </c>
+      <c r="G2">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E122" si="0">A3&amp;"."&amp;B3&amp;"@hanovernorwichschools.org"</f>
+        <v>Cathy.Niboli@hanovernorwichschools.org</v>
+      </c>
+      <c r="G3">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>Amy.Nickerson@hanovernorwichschools.org</v>
+      </c>
+      <c r="G4">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>Ian.Smith@hanovernorwichschools.org</v>
+      </c>
+      <c r="G5">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>Betty.Tedeschi@hanovernorwichschools.org</v>
+      </c>
+      <c r="G6">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>304</v>
+      </c>
+      <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>Katie.King@hanovernorwichschools.org</v>
+      </c>
+      <c r="G7">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>Vicki.Clay@hanovernorwichschools.org</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>244</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>Jonathan.Brush@hanovernorwichschools.org</v>
+      </c>
+      <c r="G9">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>Kathy.Jackson@hanovernorwichschools.org</v>
+      </c>
+      <c r="G10">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>Stephanie.Gordon@hanovernorwichschools.org</v>
+      </c>
+      <c r="G11">
+        <v>3506</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>225</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>Elizabeth.Greene@hanovernorwichschools.org</v>
+      </c>
+      <c r="G12">
+        <v>3507</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>305</v>
+      </c>
+      <c r="B13" t="s">
+        <v>306</v>
+      </c>
+      <c r="C13" t="s">
+        <v>225</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>Kara.Waters@hanovernorwichschools.org</v>
+      </c>
+      <c r="G13">
+        <v>2502</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>226</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>Todd.Bebeau@hanovernorwichschools.org</v>
+      </c>
+      <c r="G14">
+        <v>2127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D15" t="s">
+        <v>245</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>Kim.Davis@hanovernorwichschools.org</v>
+      </c>
+      <c r="G15">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>226</v>
+      </c>
+      <c r="D16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>Michael.Jackson@hanovernorwichschools.org</v>
+      </c>
+      <c r="G16">
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>226</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>Jennifer.Quevedo@hanovernorwichschools.org</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>226</v>
+      </c>
+      <c r="D18" t="s">
+        <v>247</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>Missie.Rodriquez@hanovernorwichschools.org</v>
+      </c>
+      <c r="G18">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>227</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>Ford.Daley@hanovernorwichschools.org</v>
+      </c>
+      <c r="G19">
+        <v>2132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>227</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>Bridgid.Stiller@hanovernorwichschools.org</v>
+      </c>
+      <c r="G20">
+        <v>2514</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>228</v>
+      </c>
+      <c r="D21" t="s">
+        <v>248</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="0"/>
+        <v>Dick.Lloyda@hanovernorwichschools.org</v>
+      </c>
+      <c r="G21">
+        <v>2118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" t="s">
+        <v>229</v>
+      </c>
+      <c r="D22" t="s">
+        <v>249</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="0"/>
+        <v>Carol.Ahern@hanovernorwichschools.org</v>
+      </c>
+      <c r="G22">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>229</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="0"/>
+        <v>Andrea.Alsup@hanovernorwichschools.org</v>
+      </c>
+      <c r="F23" t="s">
+        <v>260</v>
+      </c>
+      <c r="G23">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>229</v>
+      </c>
+      <c r="D24" t="s">
+        <v>250</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="0"/>
+        <v>Harrison.Bourne@hanovernorwichschools.org</v>
+      </c>
+      <c r="F24" t="s">
+        <v>261</v>
+      </c>
+      <c r="G24">
+        <v>2203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>229</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="0"/>
+        <v>Lynn.Ceplikas@hanovernorwichschools.org</v>
+      </c>
+      <c r="G25">
+        <v>2204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>229</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>Tanya.Cluff@hanovernorwichschools.org</v>
+      </c>
+      <c r="G26">
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>229</v>
+      </c>
+      <c r="E27" t="s">
+        <v>300</v>
+      </c>
+      <c r="F27" t="s">
+        <v>262</v>
+      </c>
+      <c r="G27">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" t="s">
+        <v>229</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="0"/>
+        <v>Anna.Gado@hanovernorwichschools.org</v>
+      </c>
+      <c r="G28">
+        <v>2207</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" t="s">
+        <v>229</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="0"/>
+        <v>Brian.Glenney@hanovernorwichschools.org</v>
+      </c>
+      <c r="F29" t="s">
+        <v>264</v>
+      </c>
+      <c r="G29">
+        <v>2610</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" t="s">
+        <v>229</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="0"/>
+        <v>Rennie.Gundermann@hanovernorwichschools.org</v>
+      </c>
+      <c r="F30" t="s">
+        <v>265</v>
+      </c>
+      <c r="G30">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="s">
+        <v>229</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="0"/>
+        <v>Steve.Hackman@hanovernorwichschools.org</v>
+      </c>
+      <c r="F31" t="s">
+        <v>266</v>
+      </c>
+      <c r="G31">
+        <v>2209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" t="s">
+        <v>307</v>
+      </c>
+      <c r="B32" t="s">
+        <v>308</v>
+      </c>
+      <c r="C32" t="s">
+        <v>309</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="0"/>
+        <v>Shannon.Pogue@hanovernorwichschools.org</v>
+      </c>
+      <c r="G32">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
+        <v>229</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="0"/>
+        <v>Alan.Haehnel@hanovernorwichschools.org</v>
+      </c>
+      <c r="F33" t="s">
+        <v>267</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" t="s">
+        <v>229</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>Karen.Wahrenberger@hanovernorwichschools.org</v>
+      </c>
+      <c r="F34" t="s">
+        <v>268</v>
+      </c>
+      <c r="G34">
+        <v>2210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>312</v>
+      </c>
+      <c r="B35" t="s">
+        <v>313</v>
+      </c>
+      <c r="C35" t="s">
+        <v>230</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="0"/>
+        <v>Jarrod.Shaheen@hanovernorwichschools.org</v>
+      </c>
+      <c r="G35">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>310</v>
+      </c>
+      <c r="B36" t="s">
+        <v>311</v>
+      </c>
+      <c r="C36" t="s">
+        <v>230</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>Brady.Eskilson@hanovernorwichschools.org</v>
+      </c>
+      <c r="G36">
+        <v>2601</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>230</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="0"/>
+        <v>Paul.Barker@hanovernorwichschools.org</v>
+      </c>
+      <c r="F37" t="s">
+        <v>269</v>
+      </c>
+      <c r="G37">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="0"/>
+        <v>Thomas.Cochran@hanovernorwichschools.org</v>
+      </c>
+      <c r="F38" t="s">
+        <v>271</v>
+      </c>
+      <c r="G38">
+        <v>2602</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s">
+        <v>230</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="0"/>
+        <v>Maureen.Doyle@hanovernorwichschools.org</v>
+      </c>
+      <c r="F39" t="s">
+        <v>272</v>
+      </c>
+      <c r="G39">
+        <v>2608</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" t="s">
+        <v>230</v>
+      </c>
+      <c r="D40" t="s">
+        <v>250</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="0"/>
+        <v>Brian.Glenney@hanovernorwichschools.org</v>
+      </c>
+      <c r="F40" t="s">
+        <v>264</v>
+      </c>
+      <c r="G40">
+        <v>2610</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" t="s">
+        <v>230</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="0"/>
+        <v>Uwe.Goodall-Heising@hanovernorwichschools.org</v>
+      </c>
+      <c r="F41" t="s">
+        <v>273</v>
+      </c>
+      <c r="G41">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" t="s">
+        <v>230</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="0"/>
+        <v>Katrina.McCurley@hanovernorwichschools.org</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>230</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="0"/>
+        <v>Eric.Picconi@hanovernorwichschools.org</v>
+      </c>
+      <c r="F43" t="s">
+        <v>274</v>
+      </c>
+      <c r="G43">
+        <v>2605</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" t="s">
+        <v>230</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="0"/>
+        <v>Penelope.Prendergast@hanovernorwichschools.org</v>
+      </c>
+      <c r="F44" t="s">
+        <v>275</v>
+      </c>
+      <c r="G44">
+        <v>2606</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" t="s">
+        <v>230</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="0"/>
+        <v>Jean.Vigneault@hanovernorwichschools.org</v>
+      </c>
+      <c r="F45" t="s">
+        <v>276</v>
+      </c>
+      <c r="G45">
+        <v>2609</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>231</v>
+      </c>
+      <c r="D46" t="s">
+        <v>251</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="0"/>
+        <v>Joan.Townsend@hanovernorwichschools.org</v>
+      </c>
+      <c r="G46">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" t="s">
+        <v>231</v>
+      </c>
+      <c r="D47" t="s">
+        <v>252</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="0"/>
+        <v>Laurie.Harrington@hanovernorwichschools.org</v>
+      </c>
+      <c r="G47">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48" t="s">
+        <v>231</v>
+      </c>
+      <c r="D48" t="s">
+        <v>253</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="0"/>
+        <v>Thomas.Gamble@hanovernorwichschools.org</v>
+      </c>
+      <c r="G48">
+        <v>2803</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" t="s">
+        <v>11</v>
+      </c>
+      <c r="B49" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" t="s">
+        <v>231</v>
+      </c>
+      <c r="D49" t="s">
+        <v>252</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="0"/>
+        <v>Andrea.Johnstone@hanovernorwichschools.org</v>
+      </c>
+      <c r="G49">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" t="s">
+        <v>231</v>
+      </c>
+      <c r="D50" t="s">
+        <v>252</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="0"/>
+        <v>Elizabeth.Keene@hanovernorwichschools.org</v>
+      </c>
+      <c r="G50">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" t="s">
+        <v>63</v>
+      </c>
+      <c r="B51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" t="s">
+        <v>231</v>
+      </c>
+      <c r="D51" t="s">
+        <v>254</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="0"/>
+        <v>John.McCracking@hanovernorwichschools.org</v>
+      </c>
+      <c r="G51">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" t="s">
+        <v>231</v>
+      </c>
+      <c r="D52" t="s">
+        <v>255</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="0"/>
+        <v>Stacey.Smith@hanovernorwichschools.org</v>
+      </c>
+      <c r="G52">
+        <v>2107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" t="s">
+        <v>231</v>
+      </c>
+      <c r="D53" t="s">
+        <v>256</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="0"/>
+        <v>Chris.Seibel@hanovernorwichschools.org</v>
+      </c>
+      <c r="G53">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" t="s">
+        <v>105</v>
+      </c>
+      <c r="C54" t="s">
+        <v>231</v>
+      </c>
+      <c r="D54" t="s">
+        <v>252</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="0"/>
+        <v>Joseph.Stallsmith@hanovernorwichschools.org</v>
+      </c>
+      <c r="G54">
+        <v>2106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" t="s">
+        <v>232</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="0"/>
+        <v>Diane.Guarino@hanovernorwichschools.org</v>
+      </c>
+      <c r="F55" t="s">
+        <v>277</v>
+      </c>
+      <c r="G55">
+        <v>2114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" t="s">
+        <v>233</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="0"/>
+        <v>Dave.Holloway@hanovernorwichschools.org</v>
+      </c>
+      <c r="G56">
+        <v>2702</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" t="s">
+        <v>234</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="0"/>
+        <v>Cindy.Geilich@hanovernorwichschools.org</v>
+      </c>
+      <c r="G57">
+        <v>2212</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" t="s">
+        <v>235</v>
+      </c>
+      <c r="D58" t="s">
+        <v>249</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="0"/>
+        <v>Dorothy.Adams@hanovernorwichschools.org</v>
+      </c>
+      <c r="G58">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" t="s">
+        <v>235</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="0"/>
+        <v>Eve.Ermer@hanovernorwichschools.org</v>
+      </c>
+      <c r="F59" t="s">
+        <v>278</v>
+      </c>
+      <c r="G59">
+        <v>2308</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" t="s">
+        <v>87</v>
+      </c>
+      <c r="B60" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" t="s">
+        <v>235</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="0"/>
+        <v>Eric.Dennison@hanovernorwichschools.org</v>
+      </c>
+      <c r="F60" t="s">
+        <v>279</v>
+      </c>
+      <c r="G60">
+        <v>2305</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" t="s">
+        <v>117</v>
+      </c>
+      <c r="C61" t="s">
+        <v>235</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="0"/>
+        <v>John.Donnelly@hanovernorwichschools.org</v>
+      </c>
+      <c r="F61" t="s">
+        <v>280</v>
+      </c>
+      <c r="G61">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" t="s">
+        <v>119</v>
+      </c>
+      <c r="C62" t="s">
+        <v>235</v>
+      </c>
+      <c r="D62" t="s">
+        <v>250</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="0"/>
+        <v>Jeanine.King@hanovernorwichschools.org</v>
+      </c>
+      <c r="F62" t="s">
+        <v>281</v>
+      </c>
+      <c r="G62">
+        <v>2303</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="A63" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" t="s">
+        <v>120</v>
+      </c>
+      <c r="C63" t="s">
+        <v>235</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="0"/>
+        <v>Amy.Kono@hanovernorwichschools.org</v>
+      </c>
+      <c r="F63" t="s">
+        <v>282</v>
+      </c>
+      <c r="G63">
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" t="s">
+        <v>124</v>
+      </c>
+      <c r="C64" t="s">
+        <v>235</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="0"/>
+        <v>Timothy.Kurtz@hanovernorwichschools.org</v>
+      </c>
+      <c r="F64" t="s">
+        <v>283</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" t="s">
+        <v>125</v>
+      </c>
+      <c r="B65" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" t="s">
+        <v>235</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="0"/>
+        <v>Greta.Mills@hanovernorwichschools.org</v>
+      </c>
+      <c r="F65" t="s">
+        <v>284</v>
+      </c>
+      <c r="G65">
+        <v>2309</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
+      <c r="A66" t="s">
+        <v>39</v>
+      </c>
+      <c r="B66" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" t="s">
+        <v>235</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="0"/>
+        <v>Michael.Morris@hanovernorwichschools.org</v>
+      </c>
+      <c r="F66" t="s">
+        <v>285</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" t="s">
+        <v>314</v>
+      </c>
+      <c r="B67" t="s">
+        <v>315</v>
+      </c>
+      <c r="C67" t="s">
+        <v>235</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" si="0"/>
+        <v>Warren.Tucker@hanovernorwichschools.org</v>
+      </c>
+      <c r="G67">
+        <v>2301</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" t="s">
+        <v>235</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="0"/>
+        <v>Cynthia.Sanschagrin@hanovernorwichschools.org</v>
+      </c>
+      <c r="F68" t="s">
+        <v>286</v>
+      </c>
+      <c r="G68">
+        <v>2310</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69" t="s">
+        <v>130</v>
+      </c>
+      <c r="B69" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" t="s">
+        <v>236</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="0"/>
+        <v>Martha.Cassidy@hanovernorwichschools.org</v>
+      </c>
+      <c r="G69">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" t="s">
+        <v>316</v>
+      </c>
+      <c r="B70" t="s">
+        <v>219</v>
+      </c>
+      <c r="C70" t="s">
+        <v>236</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="0"/>
+        <v>Charlie .Kehler@hanovernorwichschools.org</v>
+      </c>
+      <c r="G70">
+        <v>2506</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" t="s">
+        <v>15</v>
+      </c>
+      <c r="B71" t="s">
+        <v>191</v>
+      </c>
+      <c r="C71" t="s">
+        <v>236</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="0"/>
+        <v>Amy.Carney@hanovernorwichschools.org</v>
+      </c>
+      <c r="G71">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72" t="s">
+        <v>186</v>
+      </c>
+      <c r="B72" t="s">
+        <v>317</v>
+      </c>
+      <c r="C72" t="s">
+        <v>236</v>
+      </c>
+      <c r="E72" t="s">
+        <v>301</v>
+      </c>
+      <c r="G72">
+        <v>2505</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73" t="s">
+        <v>138</v>
+      </c>
+      <c r="B73" t="s">
+        <v>139</v>
+      </c>
+      <c r="C73" t="s">
+        <v>237</v>
+      </c>
+      <c r="D73" t="s">
+        <v>249</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="0"/>
+        <v>Patty.Armstrong@hanovernorwichschools.org</v>
+      </c>
+      <c r="F73" t="s">
+        <v>287</v>
+      </c>
+      <c r="G73">
+        <v>2507</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" t="s">
+        <v>141</v>
+      </c>
+      <c r="C74" t="s">
+        <v>237</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="0"/>
+        <v>Alexander.Spivakovsky@hanovernorwichschools.org</v>
+      </c>
+      <c r="F74" t="s">
+        <v>287</v>
+      </c>
+      <c r="G74">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75" t="s">
+        <v>142</v>
+      </c>
+      <c r="B75" t="s">
+        <v>143</v>
+      </c>
+      <c r="C75" t="s">
+        <v>237</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="0"/>
+        <v>Norman.Wolfe@hanovernorwichschools.org</v>
+      </c>
+      <c r="F75" t="s">
+        <v>287</v>
+      </c>
+      <c r="G75">
+        <v>2509</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76" t="s">
+        <v>40</v>
+      </c>
+      <c r="B76" t="s">
+        <v>318</v>
+      </c>
+      <c r="C76" t="s">
+        <v>237</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="0"/>
+        <v>Jennifer.Chambers@hanovernorwichschools.org</v>
+      </c>
+      <c r="F76" t="s">
+        <v>287</v>
+      </c>
+      <c r="G76">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77" t="s">
+        <v>146</v>
+      </c>
+      <c r="B77" t="s">
+        <v>147</v>
+      </c>
+      <c r="C77" t="s">
+        <v>238</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="0"/>
+        <v>Peg.Meyer@hanovernorwichschools.org</v>
+      </c>
+      <c r="G77">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78" t="s">
+        <v>148</v>
+      </c>
+      <c r="B78" t="s">
+        <v>149</v>
+      </c>
+      <c r="C78" t="s">
+        <v>238</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="0"/>
+        <v>Candice.Nattie@hanovernorwichschools.org</v>
+      </c>
+      <c r="G78">
+        <v>2125</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79" t="s">
+        <v>27</v>
+      </c>
+      <c r="B79" t="s">
+        <v>150</v>
+      </c>
+      <c r="C79" t="s">
+        <v>238</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="0"/>
+        <v>Kathy.Bonyai@hanovernorwichschools.org</v>
+      </c>
+      <c r="G79">
+        <v>2126</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80" t="s">
+        <v>151</v>
+      </c>
+      <c r="B80" t="s">
+        <v>152</v>
+      </c>
+      <c r="C80" t="s">
+        <v>239</v>
+      </c>
+      <c r="D80" t="s">
+        <v>249</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="0"/>
+        <v>April.Doherty@hanovernorwichschools.org</v>
+      </c>
+      <c r="G80">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
+      <c r="A81" t="s">
+        <v>153</v>
+      </c>
+      <c r="B81" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" t="s">
+        <v>239</v>
+      </c>
+      <c r="D81" t="s">
+        <v>250</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="0"/>
+        <v>Dan.Falcone@hanovernorwichschools.org</v>
+      </c>
+      <c r="F81" t="s">
+        <v>289</v>
+      </c>
+      <c r="G81">
+        <v>2701</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
+      <c r="A82" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82" t="s">
+        <v>156</v>
+      </c>
+      <c r="C82" t="s">
+        <v>239</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="0"/>
+        <v>Julia.Gartner@hanovernorwichschools.org</v>
+      </c>
+      <c r="F82" t="s">
+        <v>290</v>
+      </c>
+      <c r="G82">
+        <v>2711</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
+      <c r="A83" t="s">
+        <v>157</v>
+      </c>
+      <c r="B83" t="s">
+        <v>158</v>
+      </c>
+      <c r="C83" t="s">
+        <v>239</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="0"/>
+        <v>Sally.Hair@hanovernorwichschools.org</v>
+      </c>
+      <c r="F83" t="s">
+        <v>291</v>
+      </c>
+      <c r="G83">
+        <v>2708</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
+      <c r="A84" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" t="s">
+        <v>159</v>
+      </c>
+      <c r="C84" t="s">
+        <v>239</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="0"/>
+        <v>Thomas.Hermanson@hanovernorwichschools.org</v>
+      </c>
+      <c r="F84" t="s">
+        <v>292</v>
+      </c>
+      <c r="G84">
+        <v>2704</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
+      <c r="A85" t="s">
+        <v>160</v>
+      </c>
+      <c r="B85" t="s">
+        <v>161</v>
+      </c>
+      <c r="C85" t="s">
+        <v>239</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="0"/>
+        <v>Jeannie.Kornfeld@hanovernorwichschools.org</v>
+      </c>
+      <c r="F85" t="s">
+        <v>293</v>
+      </c>
+      <c r="G85">
+        <v>2706</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
+      <c r="A86" t="s">
+        <v>164</v>
+      </c>
+      <c r="B86" t="s">
+        <v>165</v>
+      </c>
+      <c r="C86" t="s">
+        <v>239</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="0"/>
+        <v>Casey.Milender@hanovernorwichschools.org</v>
+      </c>
+      <c r="F86" t="s">
+        <v>295</v>
+      </c>
+      <c r="G86">
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
+      <c r="A87" t="s">
+        <v>63</v>
+      </c>
+      <c r="B87" t="s">
+        <v>166</v>
+      </c>
+      <c r="C87" t="s">
+        <v>239</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="0"/>
+        <v>John.Phipps@hanovernorwichschools.org</v>
+      </c>
+      <c r="F87" t="s">
+        <v>296</v>
+      </c>
+      <c r="G87">
+        <v>2710</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
+      <c r="A88" t="s">
+        <v>319</v>
+      </c>
+      <c r="B88" t="s">
+        <v>320</v>
+      </c>
+      <c r="C88" t="s">
+        <v>239</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="0"/>
+        <v>Rachael.DiGiovanni@hanovernorwichschools.org</v>
+      </c>
+      <c r="G88">
+        <v>2707</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
+      <c r="A89" t="s">
+        <v>167</v>
+      </c>
+      <c r="B89" t="s">
+        <v>168</v>
+      </c>
+      <c r="C89" t="s">
+        <v>239</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="0"/>
+        <v>Maryann.Postans@hanovernorwichschools.org</v>
+      </c>
+      <c r="F89" t="s">
+        <v>297</v>
+      </c>
+      <c r="G89">
+        <v>2705</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
+      <c r="A90" t="s">
+        <v>169</v>
+      </c>
+      <c r="B90" t="s">
+        <v>170</v>
+      </c>
+      <c r="C90" t="s">
+        <v>240</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="0"/>
+        <v>Tim.Berube@hanovernorwichschools.org</v>
+      </c>
+      <c r="G90">
+        <v>2508</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
+      <c r="A91" t="s">
+        <v>171</v>
+      </c>
+      <c r="B91" t="s">
+        <v>172</v>
+      </c>
+      <c r="C91" t="s">
+        <v>240</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="0"/>
+        <v>Margaret.Caldwell@hanovernorwichschools.org</v>
+      </c>
+      <c r="G91">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
+      <c r="A92" t="s">
+        <v>173</v>
+      </c>
+      <c r="B92" t="s">
+        <v>174</v>
+      </c>
+      <c r="C92" t="s">
+        <v>240</v>
+      </c>
+      <c r="D92" t="s">
+        <v>249</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="0"/>
+        <v>Teresa.Drelick@hanovernorwichschools.org</v>
+      </c>
+      <c r="G92">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
+      <c r="A93" t="s">
+        <v>175</v>
+      </c>
+      <c r="B93" t="s">
+        <v>176</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="0"/>
+        <v>Seth.Goodwin@hanovernorwichschools.org</v>
+      </c>
+      <c r="F93" t="s">
+        <v>288</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
+      <c r="A94" t="s">
+        <v>177</v>
+      </c>
+      <c r="B94" t="s">
+        <v>178</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="0"/>
+        <v>Doug.Jenisch@hanovernorwichschools.org</v>
+      </c>
+      <c r="G94">
+        <v>2404</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
+      <c r="A95" t="s">
+        <v>179</v>
+      </c>
+      <c r="B95" t="s">
+        <v>180</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E95" t="s">
+        <v>302</v>
+      </c>
+      <c r="G95">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
+      <c r="A96" t="s">
+        <v>181</v>
+      </c>
+      <c r="B96" t="s">
+        <v>182</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E96" t="s">
+        <v>303</v>
+      </c>
+      <c r="G96">
+        <v>2405</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
+      <c r="A97" t="s">
+        <v>31</v>
+      </c>
+      <c r="B97" t="s">
+        <v>183</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="0"/>
+        <v>Elizabeth.Murray@hanovernorwichschools.org</v>
+      </c>
+      <c r="G97">
+        <v>2406</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
+      <c r="A98" t="s">
+        <v>184</v>
+      </c>
+      <c r="B98" t="s">
+        <v>185</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="0"/>
+        <v>Matt.Prince@hanovernorwichschools.org</v>
+      </c>
+      <c r="G98">
+        <v>2407</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
+      <c r="A99" t="s">
+        <v>322</v>
+      </c>
+      <c r="B99" t="s">
+        <v>323</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="0"/>
+        <v>Colin.Tindall@hanovernorwichschools.org</v>
+      </c>
+      <c r="G99">
+        <v>2404</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
+      <c r="A100" t="s">
+        <v>186</v>
+      </c>
+      <c r="B100" t="s">
+        <v>187</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D100" t="s">
+        <v>321</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="0"/>
+        <v>Julie.Stevenson@hanovernorwichschools.org</v>
+      </c>
+      <c r="G100">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
+      <c r="A101" t="s">
+        <v>324</v>
+      </c>
+      <c r="B101" t="s">
+        <v>325</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D101" t="s">
+        <v>249</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="0"/>
+        <v>Becky.French@hanovernorwichschools.org</v>
+      </c>
+      <c r="G101">
+        <v>2603</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
+      <c r="A102" t="s">
+        <v>15</v>
+      </c>
+      <c r="B102" t="s">
+        <v>202</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E102" t="str">
+        <f t="shared" si="0"/>
+        <v>Amy.Good@hanovernorwichschools.org</v>
+      </c>
+      <c r="G102">
+        <v>2802</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
+      <c r="A103" t="s">
+        <v>181</v>
+      </c>
+      <c r="B103" t="s">
+        <v>192</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E103" t="str">
+        <f t="shared" si="0"/>
+        <v>William.Chappelle@hanovernorwichschools.org</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
+      <c r="A104" t="s">
+        <v>193</v>
+      </c>
+      <c r="B104" t="s">
+        <v>194</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E104" t="str">
+        <f t="shared" si="0"/>
+        <v>Dale.Cloutier@hanovernorwichschools.org</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
+      <c r="A105" t="s">
+        <v>171</v>
+      </c>
+      <c r="B105" t="s">
+        <v>195</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E105" t="str">
+        <f t="shared" si="0"/>
+        <v>Margaret.Bragg@hanovernorwichschools.org</v>
+      </c>
+      <c r="G105">
+        <v>3512</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
+      <c r="A106" t="s">
+        <v>39</v>
+      </c>
+      <c r="B106" t="s">
+        <v>196</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E106" t="str">
+        <f t="shared" si="0"/>
+        <v>Michael.Callanan@hanovernorwichschools.org</v>
+      </c>
+      <c r="G106">
+        <v>3511</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
+      <c r="A107" t="s">
+        <v>197</v>
+      </c>
+      <c r="B107" t="s">
+        <v>198</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E107" t="str">
+        <f t="shared" si="0"/>
+        <v>Ellen.Clattenberg@hanovernorwichschools.org</v>
+      </c>
+      <c r="G107">
+        <v>2802</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
+      <c r="A108" t="s">
+        <v>199</v>
+      </c>
+      <c r="B108" t="s">
+        <v>200</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E108" t="str">
+        <f t="shared" si="0"/>
+        <v>Sharen.Conner@hanovernorwichschools.org</v>
+      </c>
+      <c r="G108">
+        <v>2801</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
+      <c r="A109" t="s">
+        <v>201</v>
+      </c>
+      <c r="B109" t="s">
+        <v>116</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E109" t="str">
+        <f t="shared" si="0"/>
+        <v>Cathleen.Dennison@hanovernorwichschools.org</v>
+      </c>
+      <c r="G109">
+        <v>3516</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
+      <c r="A110" t="s">
+        <v>15</v>
+      </c>
+      <c r="B110" t="s">
+        <v>202</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E110" t="str">
+        <f t="shared" si="0"/>
+        <v>Amy.Good@hanovernorwichschools.org</v>
+      </c>
+      <c r="G110">
+        <v>3510</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
+      <c r="A111" t="s">
+        <v>203</v>
+      </c>
+      <c r="B111" t="s">
+        <v>204</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E111" t="str">
+        <f t="shared" si="0"/>
+        <v>Randi.Hallarman@hanovernorwichschools.org</v>
+      </c>
+      <c r="G111">
+        <v>2805</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
+      <c r="A112" t="s">
+        <v>205</v>
+      </c>
+      <c r="B112" t="s">
+        <v>206</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D112" t="s">
+        <v>257</v>
+      </c>
+      <c r="E112" t="str">
+        <f t="shared" si="0"/>
+        <v>Deborah.Kennedy@hanovernorwichschools.org</v>
+      </c>
+      <c r="G112">
+        <v>2808</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
+      <c r="A113" t="s">
+        <v>207</v>
+      </c>
+      <c r="B113" t="s">
+        <v>208</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E113" t="str">
+        <f t="shared" si="0"/>
+        <v>Judy.McLure@hanovernorwichschools.org</v>
+      </c>
+      <c r="G113">
+        <v>2503</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
+      <c r="A114" t="s">
+        <v>209</v>
+      </c>
+      <c r="B114" t="s">
+        <v>210</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E114" t="str">
+        <f t="shared" si="0"/>
+        <v>Melissa.Minsberg@hanovernorwichschools.org</v>
+      </c>
+      <c r="G114">
+        <v>2807</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
+      <c r="A115" t="s">
+        <v>211</v>
+      </c>
+      <c r="B115" t="s">
+        <v>212</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E115" t="str">
+        <f t="shared" si="0"/>
+        <v>Deanna.Stygles@hanovernorwichschools.org</v>
+      </c>
+      <c r="G115">
+        <v>2509</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
+      <c r="A116" t="s">
+        <v>87</v>
+      </c>
+      <c r="B116" t="s">
+        <v>213</v>
+      </c>
+      <c r="C116">
+        <v>504</v>
+      </c>
+      <c r="E116" t="str">
+        <f t="shared" si="0"/>
+        <v>Eric.Richardson@hanovernorwichschools.org</v>
+      </c>
+      <c r="G116">
+        <v>2808</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
+      <c r="A117" t="s">
+        <v>173</v>
+      </c>
+      <c r="B117" t="s">
+        <v>174</v>
+      </c>
+      <c r="C117">
+        <v>504</v>
+      </c>
+      <c r="E117" t="str">
+        <f t="shared" si="0"/>
+        <v>Teresa.Drelick@hanovernorwichschools.org</v>
+      </c>
+      <c r="G117">
+        <v>2401</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
+      <c r="A118" t="s">
+        <v>214</v>
+      </c>
+      <c r="B118" t="s">
+        <v>215</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D118" t="s">
+        <v>298</v>
+      </c>
+      <c r="E118" t="str">
+        <f t="shared" si="0"/>
+        <v>Rebecca.Crane@hanovernorwichschools.org</v>
+      </c>
+      <c r="G118">
+        <v>2511</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
+      <c r="A119" t="s">
+        <v>216</v>
+      </c>
+      <c r="B119" t="s">
+        <v>217</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D119" t="s">
+        <v>258</v>
+      </c>
+      <c r="E119" t="str">
+        <f t="shared" si="0"/>
+        <v>Robert.Gere@hanovernorwichschools.org</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
+      <c r="A120" t="s">
+        <v>220</v>
+      </c>
+      <c r="B120" t="s">
+        <v>221</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D120" t="s">
+        <v>259</v>
+      </c>
+      <c r="E120" t="str">
+        <f t="shared" si="0"/>
+        <v>Tammie.Patten@hanovernorwichschools.org</v>
+      </c>
+      <c r="F120" t="s">
+        <v>299</v>
+      </c>
+      <c r="G120">
+        <v>2512</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
+      <c r="A121" t="s">
+        <v>207</v>
+      </c>
+      <c r="B121" t="s">
+        <v>222</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E121" t="str">
+        <f t="shared" si="0"/>
+        <v>Judy.Bernat@hanovernorwichschools.org</v>
+      </c>
+      <c r="G121">
+        <v>2211</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
+      <c r="A122" t="s">
+        <v>223</v>
+      </c>
+      <c r="B122" t="s">
+        <v>224</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E122" t="str">
+        <f t="shared" si="0"/>
+        <v>Debby.Cromwell@hanovernorwichschools.org</v>
+      </c>
+      <c r="G122">
+        <v>2124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>